<commit_message>
Slider working, converts input to 255 base
</commit_message>
<xml_diff>
--- a/Documentation/Screen Calc.xlsx
+++ b/Documentation/Screen Calc.xlsx
@@ -524,7 +524,7 @@
   <dimension ref="A1:CC61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+      <selection activeCell="A15" sqref="A15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9842,19 +9842,19 @@
       <c r="Y39" s="13">
         <v>10</v>
       </c>
-      <c r="Z39" s="12">
-        <v>10</v>
-      </c>
-      <c r="AA39" s="12">
-        <v>10</v>
-      </c>
-      <c r="AB39" s="12">
-        <v>10</v>
-      </c>
-      <c r="AC39" s="12">
-        <v>10</v>
-      </c>
-      <c r="AD39" s="12">
+      <c r="Z39" s="13">
+        <v>10</v>
+      </c>
+      <c r="AA39" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB39" s="13">
+        <v>10</v>
+      </c>
+      <c r="AC39" s="13">
+        <v>10</v>
+      </c>
+      <c r="AD39" s="13">
         <v>10</v>
       </c>
       <c r="AE39" s="13">
@@ -9917,19 +9917,19 @@
       <c r="AX39" s="13">
         <v>10</v>
       </c>
-      <c r="AY39" s="12">
-        <v>10</v>
-      </c>
-      <c r="AZ39" s="12">
-        <v>10</v>
-      </c>
-      <c r="BA39" s="12">
-        <v>10</v>
-      </c>
-      <c r="BB39" s="12">
-        <v>10</v>
-      </c>
-      <c r="BC39" s="12">
+      <c r="AY39" s="13">
+        <v>10</v>
+      </c>
+      <c r="AZ39" s="13">
+        <v>10</v>
+      </c>
+      <c r="BA39" s="13">
+        <v>10</v>
+      </c>
+      <c r="BB39" s="13">
+        <v>10</v>
+      </c>
+      <c r="BC39" s="13">
         <v>10</v>
       </c>
       <c r="BD39" s="13">
@@ -10085,19 +10085,19 @@
       <c r="Y40" s="13">
         <v>10</v>
       </c>
-      <c r="Z40" s="12">
-        <v>10</v>
-      </c>
-      <c r="AA40" s="12">
-        <v>10</v>
-      </c>
-      <c r="AB40" s="12">
-        <v>10</v>
-      </c>
-      <c r="AC40" s="12">
-        <v>10</v>
-      </c>
-      <c r="AD40" s="12">
+      <c r="Z40" s="13">
+        <v>10</v>
+      </c>
+      <c r="AA40" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB40" s="13">
+        <v>10</v>
+      </c>
+      <c r="AC40" s="13">
+        <v>10</v>
+      </c>
+      <c r="AD40" s="13">
         <v>10</v>
       </c>
       <c r="AE40" s="13">
@@ -10160,19 +10160,19 @@
       <c r="AX40" s="13">
         <v>10</v>
       </c>
-      <c r="AY40" s="12">
-        <v>10</v>
-      </c>
-      <c r="AZ40" s="12">
-        <v>10</v>
-      </c>
-      <c r="BA40" s="12">
-        <v>10</v>
-      </c>
-      <c r="BB40" s="12">
-        <v>10</v>
-      </c>
-      <c r="BC40" s="12">
+      <c r="AY40" s="13">
+        <v>10</v>
+      </c>
+      <c r="AZ40" s="13">
+        <v>10</v>
+      </c>
+      <c r="BA40" s="13">
+        <v>10</v>
+      </c>
+      <c r="BB40" s="13">
+        <v>10</v>
+      </c>
+      <c r="BC40" s="13">
         <v>10</v>
       </c>
       <c r="BD40" s="13">
@@ -10328,19 +10328,19 @@
       <c r="Y41" s="13">
         <v>10</v>
       </c>
-      <c r="Z41" s="12">
-        <v>10</v>
-      </c>
-      <c r="AA41" s="12">
-        <v>10</v>
-      </c>
-      <c r="AB41" s="12">
-        <v>10</v>
-      </c>
-      <c r="AC41" s="12">
-        <v>10</v>
-      </c>
-      <c r="AD41" s="12">
+      <c r="Z41" s="13">
+        <v>10</v>
+      </c>
+      <c r="AA41" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB41" s="13">
+        <v>10</v>
+      </c>
+      <c r="AC41" s="13">
+        <v>10</v>
+      </c>
+      <c r="AD41" s="13">
         <v>10</v>
       </c>
       <c r="AE41" s="13">
@@ -10403,19 +10403,19 @@
       <c r="AX41" s="13">
         <v>10</v>
       </c>
-      <c r="AY41" s="12">
-        <v>10</v>
-      </c>
-      <c r="AZ41" s="12">
-        <v>10</v>
-      </c>
-      <c r="BA41" s="12">
-        <v>10</v>
-      </c>
-      <c r="BB41" s="12">
-        <v>10</v>
-      </c>
-      <c r="BC41" s="12">
+      <c r="AY41" s="13">
+        <v>10</v>
+      </c>
+      <c r="AZ41" s="13">
+        <v>10</v>
+      </c>
+      <c r="BA41" s="13">
+        <v>10</v>
+      </c>
+      <c r="BB41" s="13">
+        <v>10</v>
+      </c>
+      <c r="BC41" s="13">
         <v>10</v>
       </c>
       <c r="BD41" s="13">
@@ -10571,19 +10571,19 @@
       <c r="Y42" s="13">
         <v>10</v>
       </c>
-      <c r="Z42" s="12">
-        <v>10</v>
-      </c>
-      <c r="AA42" s="12">
-        <v>10</v>
-      </c>
-      <c r="AB42" s="12">
-        <v>10</v>
-      </c>
-      <c r="AC42" s="12">
-        <v>10</v>
-      </c>
-      <c r="AD42" s="12">
+      <c r="Z42" s="13">
+        <v>10</v>
+      </c>
+      <c r="AA42" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB42" s="13">
+        <v>10</v>
+      </c>
+      <c r="AC42" s="13">
+        <v>10</v>
+      </c>
+      <c r="AD42" s="13">
         <v>10</v>
       </c>
       <c r="AE42" s="13">
@@ -10646,19 +10646,19 @@
       <c r="AX42" s="13">
         <v>10</v>
       </c>
-      <c r="AY42" s="12">
-        <v>10</v>
-      </c>
-      <c r="AZ42" s="12">
-        <v>10</v>
-      </c>
-      <c r="BA42" s="12">
-        <v>10</v>
-      </c>
-      <c r="BB42" s="12">
-        <v>10</v>
-      </c>
-      <c r="BC42" s="12">
+      <c r="AY42" s="13">
+        <v>10</v>
+      </c>
+      <c r="AZ42" s="13">
+        <v>10</v>
+      </c>
+      <c r="BA42" s="13">
+        <v>10</v>
+      </c>
+      <c r="BB42" s="13">
+        <v>10</v>
+      </c>
+      <c r="BC42" s="13">
         <v>10</v>
       </c>
       <c r="BD42" s="13">
@@ -10814,19 +10814,19 @@
       <c r="Y43" s="13">
         <v>10</v>
       </c>
-      <c r="Z43" s="12">
-        <v>10</v>
-      </c>
-      <c r="AA43" s="12">
-        <v>10</v>
-      </c>
-      <c r="AB43" s="12">
-        <v>10</v>
-      </c>
-      <c r="AC43" s="12">
-        <v>10</v>
-      </c>
-      <c r="AD43" s="12">
+      <c r="Z43" s="13">
+        <v>10</v>
+      </c>
+      <c r="AA43" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB43" s="13">
+        <v>10</v>
+      </c>
+      <c r="AC43" s="13">
+        <v>10</v>
+      </c>
+      <c r="AD43" s="13">
         <v>10</v>
       </c>
       <c r="AE43" s="13">
@@ -10889,19 +10889,19 @@
       <c r="AX43" s="13">
         <v>10</v>
       </c>
-      <c r="AY43" s="12">
-        <v>10</v>
-      </c>
-      <c r="AZ43" s="12">
-        <v>10</v>
-      </c>
-      <c r="BA43" s="12">
-        <v>10</v>
-      </c>
-      <c r="BB43" s="12">
-        <v>10</v>
-      </c>
-      <c r="BC43" s="12">
+      <c r="AY43" s="13">
+        <v>10</v>
+      </c>
+      <c r="AZ43" s="13">
+        <v>10</v>
+      </c>
+      <c r="BA43" s="13">
+        <v>10</v>
+      </c>
+      <c r="BB43" s="13">
+        <v>10</v>
+      </c>
+      <c r="BC43" s="13">
         <v>10</v>
       </c>
       <c r="BD43" s="13">
@@ -11057,19 +11057,19 @@
       <c r="Y44" s="13">
         <v>10</v>
       </c>
-      <c r="Z44" s="12">
-        <v>10</v>
-      </c>
-      <c r="AA44" s="12">
-        <v>10</v>
-      </c>
-      <c r="AB44" s="12">
-        <v>10</v>
-      </c>
-      <c r="AC44" s="12">
-        <v>10</v>
-      </c>
-      <c r="AD44" s="12">
+      <c r="Z44" s="13">
+        <v>10</v>
+      </c>
+      <c r="AA44" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB44" s="13">
+        <v>10</v>
+      </c>
+      <c r="AC44" s="13">
+        <v>10</v>
+      </c>
+      <c r="AD44" s="13">
         <v>10</v>
       </c>
       <c r="AE44" s="13">
@@ -11132,19 +11132,19 @@
       <c r="AX44" s="13">
         <v>10</v>
       </c>
-      <c r="AY44" s="12">
-        <v>10</v>
-      </c>
-      <c r="AZ44" s="12">
-        <v>10</v>
-      </c>
-      <c r="BA44" s="12">
-        <v>10</v>
-      </c>
-      <c r="BB44" s="12">
-        <v>10</v>
-      </c>
-      <c r="BC44" s="12">
+      <c r="AY44" s="13">
+        <v>10</v>
+      </c>
+      <c r="AZ44" s="13">
+        <v>10</v>
+      </c>
+      <c r="BA44" s="13">
+        <v>10</v>
+      </c>
+      <c r="BB44" s="13">
+        <v>10</v>
+      </c>
+      <c r="BC44" s="13">
         <v>10</v>
       </c>
       <c r="BD44" s="13">
@@ -11300,19 +11300,19 @@
       <c r="Y45" s="13">
         <v>10</v>
       </c>
-      <c r="Z45" s="12">
-        <v>10</v>
-      </c>
-      <c r="AA45" s="12">
-        <v>10</v>
-      </c>
-      <c r="AB45" s="12">
-        <v>10</v>
-      </c>
-      <c r="AC45" s="12">
-        <v>10</v>
-      </c>
-      <c r="AD45" s="12">
+      <c r="Z45" s="13">
+        <v>10</v>
+      </c>
+      <c r="AA45" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB45" s="13">
+        <v>10</v>
+      </c>
+      <c r="AC45" s="13">
+        <v>10</v>
+      </c>
+      <c r="AD45" s="13">
         <v>10</v>
       </c>
       <c r="AE45" s="13">
@@ -11375,19 +11375,19 @@
       <c r="AX45" s="13">
         <v>10</v>
       </c>
-      <c r="AY45" s="12">
-        <v>10</v>
-      </c>
-      <c r="AZ45" s="12">
-        <v>10</v>
-      </c>
-      <c r="BA45" s="12">
-        <v>10</v>
-      </c>
-      <c r="BB45" s="12">
-        <v>10</v>
-      </c>
-      <c r="BC45" s="12">
+      <c r="AY45" s="13">
+        <v>10</v>
+      </c>
+      <c r="AZ45" s="13">
+        <v>10</v>
+      </c>
+      <c r="BA45" s="13">
+        <v>10</v>
+      </c>
+      <c r="BB45" s="13">
+        <v>10</v>
+      </c>
+      <c r="BC45" s="13">
         <v>10</v>
       </c>
       <c r="BD45" s="13">
@@ -11543,19 +11543,19 @@
       <c r="Y46" s="13">
         <v>10</v>
       </c>
-      <c r="Z46" s="12">
-        <v>10</v>
-      </c>
-      <c r="AA46" s="12">
-        <v>10</v>
-      </c>
-      <c r="AB46" s="12">
-        <v>10</v>
-      </c>
-      <c r="AC46" s="12">
-        <v>10</v>
-      </c>
-      <c r="AD46" s="12">
+      <c r="Z46" s="13">
+        <v>10</v>
+      </c>
+      <c r="AA46" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB46" s="13">
+        <v>10</v>
+      </c>
+      <c r="AC46" s="13">
+        <v>10</v>
+      </c>
+      <c r="AD46" s="13">
         <v>10</v>
       </c>
       <c r="AE46" s="13">
@@ -11618,19 +11618,19 @@
       <c r="AX46" s="13">
         <v>10</v>
       </c>
-      <c r="AY46" s="12">
-        <v>10</v>
-      </c>
-      <c r="AZ46" s="12">
-        <v>10</v>
-      </c>
-      <c r="BA46" s="12">
-        <v>10</v>
-      </c>
-      <c r="BB46" s="12">
-        <v>10</v>
-      </c>
-      <c r="BC46" s="12">
+      <c r="AY46" s="13">
+        <v>10</v>
+      </c>
+      <c r="AZ46" s="13">
+        <v>10</v>
+      </c>
+      <c r="BA46" s="13">
+        <v>10</v>
+      </c>
+      <c r="BB46" s="13">
+        <v>10</v>
+      </c>
+      <c r="BC46" s="13">
         <v>10</v>
       </c>
       <c r="BD46" s="13">
@@ -11786,19 +11786,19 @@
       <c r="Y47" s="13">
         <v>10</v>
       </c>
-      <c r="Z47" s="12">
-        <v>10</v>
-      </c>
-      <c r="AA47" s="12">
-        <v>10</v>
-      </c>
-      <c r="AB47" s="12">
-        <v>10</v>
-      </c>
-      <c r="AC47" s="12">
-        <v>10</v>
-      </c>
-      <c r="AD47" s="12">
+      <c r="Z47" s="13">
+        <v>10</v>
+      </c>
+      <c r="AA47" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB47" s="13">
+        <v>10</v>
+      </c>
+      <c r="AC47" s="13">
+        <v>10</v>
+      </c>
+      <c r="AD47" s="13">
         <v>10</v>
       </c>
       <c r="AE47" s="13">
@@ -11861,19 +11861,19 @@
       <c r="AX47" s="13">
         <v>10</v>
       </c>
-      <c r="AY47" s="12">
-        <v>10</v>
-      </c>
-      <c r="AZ47" s="12">
-        <v>10</v>
-      </c>
-      <c r="BA47" s="12">
-        <v>10</v>
-      </c>
-      <c r="BB47" s="12">
-        <v>10</v>
-      </c>
-      <c r="BC47" s="12">
+      <c r="AY47" s="13">
+        <v>10</v>
+      </c>
+      <c r="AZ47" s="13">
+        <v>10</v>
+      </c>
+      <c r="BA47" s="13">
+        <v>10</v>
+      </c>
+      <c r="BB47" s="13">
+        <v>10</v>
+      </c>
+      <c r="BC47" s="13">
         <v>10</v>
       </c>
       <c r="BD47" s="13">

</xml_diff>